<commit_message>
add receipt_number in aservice88
</commit_message>
<xml_diff>
--- a/aservice88/tmplts/E1.xlsx
+++ b/aservice88/tmplts/E1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smdlkhn/PycharmProjects/cifrotech_webapp_/aservice88/tmplts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cifrotech\PycharmProjects\cifrotech_webapp_\aservice88\tmplts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A32563-F648-0649-9DB6-888555D731DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50A66A5-8B95-4C0C-907A-6AC3A20D3F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25440" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>т. +7(978)7156486</t>
   </si>
   <si>
-    <t>ТОВАРНЫЙ ЧЕК № 40468</t>
-  </si>
-  <si>
     <t>Наименование и серийный номер</t>
   </si>
   <si>
@@ -88,13 +85,16 @@
   </si>
   <si>
     <t>Итого (сумма прописью): {{ total_by_words }} руб 00 коп</t>
+  </si>
+  <si>
+    <t>ТОВАРНЫЙ ЧЕК № {{ receipt_number }}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial Cyr"/>
@@ -615,19 +615,19 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.5" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="47.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.75" customHeight="1">
+    <row r="1" spans="1:5" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -636,7 +636,7 @@
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
     </row>
-    <row r="2" spans="1:5" ht="17.75" customHeight="1">
+    <row r="2" spans="1:5" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -645,7 +645,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" ht="17.75" customHeight="1">
+    <row r="3" spans="1:5" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
@@ -654,7 +654,7 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:5" ht="17.75" customHeight="1">
+    <row r="4" spans="1:5" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
@@ -663,157 +663,157 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" ht="17.75" customHeight="1">
+    <row r="5" spans="1:5" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:5" ht="15.5" customHeight="1">
+    <row r="6" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="1:5" ht="17" customHeight="1">
+    <row r="7" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="32.25" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30.75" customHeight="1">
+    </row>
+    <row r="9" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.5" customHeight="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="15.5" customHeight="1">
+    <row r="11" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
     </row>
-    <row r="12" spans="1:5" ht="15.5" customHeight="1">
+    <row r="12" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="15.5" customHeight="1">
+    <row r="13" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:5" ht="23" customHeight="1">
+    <row r="14" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="23" customHeight="1">
+    <row r="15" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5" ht="23" customHeight="1">
+    <row r="16" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" ht="15.5" customHeight="1">
+    <row r="17" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="15.5" customHeight="1">
+    <row r="18" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" ht="7.75" customHeight="1">
+    <row r="19" spans="1:5" ht="7.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" ht="15.5" customHeight="1">
+    <row r="20" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
     </row>
-    <row r="21" spans="1:5" ht="15.5" customHeight="1">
+    <row r="21" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -854,7 +854,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -868,7 +868,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>